<commit_message>
Cambio de cadena de conexion
Cambio de cadena de conexion
</commit_message>
<xml_diff>
--- a/Requerimientos DVGP.xlsx
+++ b/Requerimientos DVGP.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\DGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Projecto\DGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8730" windowHeight="5895" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8730" windowHeight="5895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glosario de terminos" sheetId="3" r:id="rId1"/>
     <sheet name="Requerimiento" sheetId="1" r:id="rId2"/>
     <sheet name="Diseño Modulo Despacho" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -310,7 +310,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -538,28 +538,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A4:C29" totalsRowShown="0">
-  <autoFilter ref="A4:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A4:C29" totalsRowShown="0">
+  <autoFilter ref="A4:C29" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Titulo"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="0"/>
-    <tableColumn id="3" name="observación"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Titulo"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="observación"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A4:G27" totalsRowShown="0">
-  <autoFilter ref="A4:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A4:G27" totalsRowShown="0">
+  <autoFilter ref="A4:G27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="ítem"/>
-    <tableColumn id="6" name="Source"/>
-    <tableColumn id="2" name="Titulo"/>
-    <tableColumn id="3" name="Descripción"/>
-    <tableColumn id="4" name="Prioridad"/>
-    <tableColumn id="5" name="sprint"/>
-    <tableColumn id="7" name="Horas Estimadas"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ítem"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Source"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Titulo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Descripción"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Prioridad"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="sprint"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Horas Estimadas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -827,7 +827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1067,11 +1067,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,8 +1370,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
-    <hyperlink ref="I5" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1381,7 +1381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">

</xml_diff>